<commit_message>
Carga los datos de servicios soap en la tabla
</commit_message>
<xml_diff>
--- a/DataDriven/DataDrivenFBServ.xlsx
+++ b/DataDriven/DataDrivenFBServ.xlsx
@@ -446,7 +446,7 @@
   <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,41 +531,41 @@
         <v>1</v>
       </c>
       <c r="B2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2" s="2">
         <f>A2+B2</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D2" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F2" s="2">
         <f>D2-E2</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G2" s="2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H2" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I2" s="2">
         <f>G2*H2</f>
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="J2" s="2">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="K2" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L2" s="2">
         <f>J2/K2</f>
-        <v>1</v>
+        <v>0.875</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>